<commit_message>
Corrected info concerning Mary Ann Cohchran
</commit_message>
<xml_diff>
--- a/InfoTableData.xlsx
+++ b/InfoTableData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4460" uniqueCount="851">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4457" uniqueCount="857">
   <si>
     <t>bio</t>
   </si>
@@ -2155,9 +2155,6 @@
     <t>Adolfina_x000D_</t>
   </si>
   <si>
-    <t>Richard J Falkman_x000D_</t>
-  </si>
-  <si>
     <t>1680 – January 1751_x000D__x000D_</t>
   </si>
   <si>
@@ -2567,6 +2564,27 @@
   </si>
   <si>
     <t>18 Oct 1965</t>
+  </si>
+  <si>
+    <t>Mary Ann</t>
+  </si>
+  <si>
+    <t>Mary Ann Cochran.txt</t>
+  </si>
+  <si>
+    <t>Cleveland, Oh.</t>
+  </si>
+  <si>
+    <t>07 Jan 1946 - 30 Oct 2016</t>
+  </si>
+  <si>
+    <t>Ernest J Cochran</t>
+  </si>
+  <si>
+    <t>Helen Elizabeth Seibert</t>
+  </si>
+  <si>
+    <t>Mary Ann Cochran.jpg</t>
   </si>
 </sst>
 </file>
@@ -2945,9 +2963,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AK134"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A117" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E104" sqref="E104"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A103" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R125" sqref="R125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -2991,7 +3009,7 @@
         <v>2</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="H1" t="s">
         <v>13</v>
@@ -3086,7 +3104,7 @@
     </row>
     <row r="2" spans="1:37">
       <c r="A2" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="B2" t="s">
         <v>678</v>
@@ -3098,10 +3116,10 @@
         <v>36</v>
       </c>
       <c r="E2" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="G2" s="2">
         <v>775</v>
@@ -3128,7 +3146,7 @@
         <v>36</v>
       </c>
       <c r="O2" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="P2" t="s">
         <v>36</v>
@@ -3211,7 +3229,7 @@
         <v>480</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="G3" s="2">
         <v>1560</v>
@@ -3324,7 +3342,7 @@
         <v>151</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="G4" s="2">
         <v>1590</v>
@@ -3437,7 +3455,7 @@
         <v>158</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="G5" s="2">
         <v>1600</v>
@@ -3550,7 +3568,7 @@
         <v>578</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="G6" s="2">
         <v>1620</v>
@@ -3660,10 +3678,10 @@
         <v>36</v>
       </c>
       <c r="E7" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="G7" s="2">
         <v>1625</v>
@@ -3773,7 +3791,7 @@
         <v>504</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="G8" s="2">
         <v>1625</v>
@@ -3999,7 +4017,7 @@
         <v>502</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="G10" s="2">
         <v>1630</v>
@@ -4112,7 +4130,7 @@
         <v>513</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="G11" s="2">
         <v>1630</v>
@@ -4225,7 +4243,7 @@
         <v>453</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="G12" s="2">
         <v>1635</v>
@@ -4338,7 +4356,7 @@
         <v>294</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="G13" s="2">
         <v>1640</v>
@@ -4451,7 +4469,7 @@
         <v>302</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="G14" s="2">
         <v>1650</v>
@@ -4564,7 +4582,7 @@
         <v>319</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="G15" s="2">
         <v>1650</v>
@@ -4677,7 +4695,7 @@
         <v>297</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="G16" s="2">
         <v>1650</v>
@@ -4790,7 +4808,7 @@
         <v>317</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="G17" s="2">
         <v>1660</v>
@@ -4903,7 +4921,7 @@
         <v>499</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="G18" s="2">
         <v>1660</v>
@@ -5016,7 +5034,7 @@
         <v>450</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="G19" s="2">
         <v>1665</v>
@@ -5129,7 +5147,7 @@
         <v>298</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="G20" s="2">
         <v>1670</v>
@@ -5242,7 +5260,7 @@
         <v>470</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="G21" s="2">
         <v>1670</v>
@@ -5355,7 +5373,7 @@
         <v>570</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="G22" s="2">
         <v>1670</v>
@@ -5468,7 +5486,7 @@
         <v>580</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="G23" s="2">
         <v>1670</v>
@@ -5581,7 +5599,7 @@
         <v>158</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="G24" s="2">
         <v>1672</v>
@@ -5694,7 +5712,7 @@
         <v>474</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="G25" s="2">
         <v>1674</v>
@@ -5804,7 +5822,7 @@
         <v>240</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="G26" s="2">
         <v>1675</v>
@@ -5917,7 +5935,7 @@
         <v>238</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="G27" s="2">
         <v>1675</v>
@@ -6030,7 +6048,7 @@
         <v>311</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="G28" s="2">
         <v>1676</v>
@@ -6143,7 +6161,7 @@
         <v>645</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="G29" s="2">
         <v>1676</v>
@@ -6236,7 +6254,7 @@
         <v>36</v>
       </c>
       <c r="AK29" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="30" spans="1:37">
@@ -6256,7 +6274,7 @@
         <v>313</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="G30" s="2">
         <v>1680</v>
@@ -6369,7 +6387,7 @@
         <v>483</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="G31" s="2">
         <v>1690</v>
@@ -6595,7 +6613,7 @@
         <v>575</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="G33" s="2">
         <v>1697</v>
@@ -6708,7 +6726,7 @@
         <v>189</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="G34" s="2">
         <v>1700</v>
@@ -6821,7 +6839,7 @@
         <v>604</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="G35" s="2">
         <v>1700</v>
@@ -6934,7 +6952,7 @@
         <v>568</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="G36" s="2">
         <v>1700</v>
@@ -7386,7 +7404,7 @@
         <v>320</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="G40" s="2">
         <v>1719</v>
@@ -7612,7 +7630,7 @@
         <v>632</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="G42" s="2">
         <v>1737</v>
@@ -7725,7 +7743,7 @@
         <v>474</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="G43" s="2">
         <v>1738</v>
@@ -7951,7 +7969,7 @@
         <v>607</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="G45" s="2">
         <v>1750</v>
@@ -8174,7 +8192,7 @@
         <v>448</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="G47" s="2">
         <v>1798</v>
@@ -8287,7 +8305,7 @@
         <v>251</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="G48" s="2">
         <v>1823</v>
@@ -8400,7 +8418,7 @@
         <v>228</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="G49" s="2">
         <v>1825</v>
@@ -8513,7 +8531,7 @@
         <v>253</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="G50" s="2">
         <v>1830</v>
@@ -8626,7 +8644,7 @@
         <v>273</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="G51" s="2">
         <v>1830</v>
@@ -8965,7 +8983,7 @@
         <v>276</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="G54" s="2">
         <v>1830</v>
@@ -9051,7 +9069,7 @@
         <v>639</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="G55" s="2">
         <v>1834</v>
@@ -9155,13 +9173,13 @@
         <v>478</v>
       </c>
       <c r="C56" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="D56" t="s">
         <v>36</v>
       </c>
       <c r="E56" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="F56" s="2" t="s">
         <v>540</v>
@@ -9203,7 +9221,7 @@
         <v>36</v>
       </c>
       <c r="S56" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="T56" t="s">
         <v>146</v>
@@ -9378,10 +9396,10 @@
         <v>133</v>
       </c>
       <c r="C58" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="D58" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="E58" t="s">
         <v>108</v>
@@ -9830,7 +9848,7 @@
         <v>187</v>
       </c>
       <c r="C62" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="D62" t="s">
         <v>36</v>
@@ -10895,7 +10913,7 @@
         <v>36</v>
       </c>
       <c r="S71" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="T71" t="s">
         <v>146</v>
@@ -11421,7 +11439,7 @@
         <v>243</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="G76" s="2">
         <v>1874</v>
@@ -12099,7 +12117,7 @@
         <v>447</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="G82" s="2">
         <v>1891</v>
@@ -12480,7 +12498,7 @@
         <v>149</v>
       </c>
       <c r="T85" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="U85" t="s">
         <v>36</v>
@@ -12887,7 +12905,7 @@
         <v>36</v>
       </c>
       <c r="E89" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="F89" s="2" t="s">
         <v>373</v>
@@ -13229,7 +13247,7 @@
         <v>66</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="G92" s="2">
         <v>1915</v>
@@ -13440,16 +13458,16 @@
         <v>98</v>
       </c>
       <c r="C94" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="D94" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="E94" t="s">
         <v>84</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="G94" s="2">
         <v>1918</v>
@@ -13464,7 +13482,7 @@
         <v>435</v>
       </c>
       <c r="K94" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="L94" t="s">
         <v>75</v>
@@ -13562,7 +13580,7 @@
         <v>41</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="G95" s="2">
         <v>1921</v>
@@ -13770,7 +13788,7 @@
     </row>
     <row r="97" spans="1:37">
       <c r="A97" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="B97" t="s">
         <v>387</v>
@@ -13779,13 +13797,13 @@
         <v>36</v>
       </c>
       <c r="D97" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="E97" t="s">
         <v>213</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="G97" s="2">
         <v>1935</v>
@@ -14005,34 +14023,34 @@
         <v>124</v>
       </c>
       <c r="E99" s="3" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="G99" s="2">
         <v>1937</v>
       </c>
       <c r="H99" t="s">
+        <v>796</v>
+      </c>
+      <c r="I99" t="s">
         <v>797</v>
       </c>
-      <c r="I99" t="s">
-        <v>798</v>
-      </c>
       <c r="L99" t="s">
+        <v>803</v>
+      </c>
+      <c r="M99" t="s">
         <v>804</v>
       </c>
-      <c r="M99" t="s">
+      <c r="N99" t="s">
         <v>805</v>
       </c>
-      <c r="N99" t="s">
+      <c r="O99" t="s">
         <v>806</v>
       </c>
-      <c r="O99" t="s">
-        <v>807</v>
-      </c>
       <c r="P99" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="Q99" t="s">
         <v>353</v>
@@ -14282,31 +14300,31 @@
         <v>675</v>
       </c>
       <c r="B102" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="C102" t="s">
         <v>89</v>
       </c>
       <c r="E102" s="3" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="G102" s="2">
         <v>1942</v>
       </c>
       <c r="H102" t="s">
+        <v>796</v>
+      </c>
+      <c r="I102" t="s">
         <v>797</v>
       </c>
-      <c r="I102" t="s">
-        <v>798</v>
-      </c>
       <c r="O102" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="P102" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="Q102" t="s">
         <v>353</v>
@@ -14332,7 +14350,7 @@
         <v>98</v>
       </c>
       <c r="C103" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="D103" t="s">
         <v>400</v>
@@ -14451,10 +14469,10 @@
         <v>390</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="G104" s="2" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="H104" t="s">
         <v>75</v>
@@ -14677,7 +14695,7 @@
         <v>624</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="G106" s="2">
         <v>1945</v>
@@ -14778,7 +14796,7 @@
         <v>197</v>
       </c>
       <c r="B107" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="C107" t="s">
         <v>36</v>
@@ -14790,7 +14808,7 @@
         <v>193</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="G107" s="2">
         <v>1946</v>
@@ -14802,7 +14820,7 @@
         <v>121</v>
       </c>
       <c r="J107" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="K107" t="s">
         <v>103</v>
@@ -14817,7 +14835,7 @@
         <v>36</v>
       </c>
       <c r="S107" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="T107" t="s">
         <v>36</v>
@@ -14927,7 +14945,7 @@
         <v>78</v>
       </c>
       <c r="S108" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="T108" t="s">
         <v>333</v>
@@ -15001,7 +15019,7 @@
         <v>348</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="G109" s="2">
         <v>1946</v>
@@ -15019,10 +15037,10 @@
         <v>345</v>
       </c>
       <c r="L109" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="O109" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="P109" t="s">
         <v>346</v>
@@ -15034,7 +15052,7 @@
         <v>78</v>
       </c>
       <c r="S109" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="T109" t="s">
         <v>263</v>
@@ -15108,7 +15126,7 @@
         <v>347</v>
       </c>
       <c r="F110" s="2" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="G110" s="2">
         <v>1946</v>
@@ -15129,16 +15147,16 @@
         <v>353</v>
       </c>
       <c r="P110" t="s">
+        <v>799</v>
+      </c>
+      <c r="Q110" t="s">
         <v>800</v>
-      </c>
-      <c r="Q110" t="s">
-        <v>801</v>
       </c>
       <c r="R110" t="s">
         <v>78</v>
       </c>
       <c r="S110" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="T110" t="s">
         <v>263</v>
@@ -15313,7 +15331,7 @@
         <v>260</v>
       </c>
       <c r="B112" t="s">
-        <v>123</v>
+        <v>850</v>
       </c>
       <c r="C112" t="s">
         <v>36</v>
@@ -15325,22 +15343,22 @@
         <v>261</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>256</v>
+        <v>853</v>
       </c>
       <c r="G112" s="2">
-        <v>1947</v>
+        <v>1946</v>
       </c>
       <c r="H112" t="s">
-        <v>713</v>
+        <v>854</v>
       </c>
       <c r="I112" t="s">
-        <v>41</v>
+        <v>855</v>
       </c>
       <c r="J112" t="s">
-        <v>36</v>
+        <v>851</v>
       </c>
       <c r="K112" t="s">
-        <v>255</v>
+        <v>852</v>
       </c>
       <c r="L112" t="s">
         <v>257</v>
@@ -15352,19 +15370,10 @@
         <v>36</v>
       </c>
       <c r="O112" t="s">
-        <v>261</v>
-      </c>
-      <c r="P112" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q112" t="s">
-        <v>76</v>
-      </c>
-      <c r="R112" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="S112" t="s">
-        <v>262</v>
+        <v>856</v>
       </c>
       <c r="T112" t="s">
         <v>263</v>
@@ -15542,7 +15551,7 @@
         <v>674</v>
       </c>
       <c r="C114" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="D114" t="s">
         <v>36</v>
@@ -15551,16 +15560,16 @@
         <v>353</v>
       </c>
       <c r="F114" s="2" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="G114" s="2">
         <v>1947</v>
       </c>
       <c r="H114" t="s">
+        <v>796</v>
+      </c>
+      <c r="I114" t="s">
         <v>797</v>
-      </c>
-      <c r="I114" t="s">
-        <v>798</v>
       </c>
       <c r="J114" t="s">
         <v>36</v>
@@ -15581,13 +15590,13 @@
         <v>76</v>
       </c>
       <c r="P114" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="Q114" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="S114" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="T114" t="s">
         <v>263</v>
@@ -15765,7 +15774,7 @@
         <v>288</v>
       </c>
       <c r="F116" s="2" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="G116" s="2">
         <v>1950</v>
@@ -15878,16 +15887,16 @@
         <v>344</v>
       </c>
       <c r="F117" s="2" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="G117" s="2">
         <v>1951</v>
       </c>
       <c r="H117" t="s">
+        <v>735</v>
+      </c>
+      <c r="I117" t="s">
         <v>736</v>
-      </c>
-      <c r="I117" t="s">
-        <v>737</v>
       </c>
       <c r="K117" t="s">
         <v>408</v>
@@ -15902,25 +15911,25 @@
         <v>137</v>
       </c>
       <c r="P117" t="s">
+        <v>821</v>
+      </c>
+      <c r="Q117" t="s">
         <v>822</v>
       </c>
-      <c r="Q117" t="s">
-        <v>823</v>
-      </c>
       <c r="S117" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="T117" t="s">
         <v>342</v>
       </c>
       <c r="U117" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="V117" t="s">
+        <v>737</v>
+      </c>
+      <c r="W117" t="s">
         <v>738</v>
-      </c>
-      <c r="W117" t="s">
-        <v>739</v>
       </c>
       <c r="X117" t="s">
         <v>343</v>
@@ -16095,16 +16104,16 @@
         <v>182</v>
       </c>
       <c r="F119" s="2" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="G119" s="2">
         <v>1957</v>
       </c>
       <c r="H119" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="I119" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="J119" t="s">
         <v>36</v>
@@ -16140,7 +16149,7 @@
         <v>414</v>
       </c>
       <c r="U119" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="V119" t="s">
         <v>263</v>
@@ -16336,7 +16345,7 @@
         <v>367</v>
       </c>
       <c r="K121" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="L121" t="s">
         <v>36</v>
@@ -16348,7 +16357,7 @@
         <v>36</v>
       </c>
       <c r="O121" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="P121" t="s">
         <v>347</v>
@@ -16431,7 +16440,7 @@
         <v>391</v>
       </c>
       <c r="F122" s="2" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="G122" s="2">
         <v>1971</v>
@@ -16529,58 +16538,58 @@
     </row>
     <row r="123" spans="1:37">
       <c r="A123" t="s">
+        <v>778</v>
+      </c>
+      <c r="B123" t="s">
         <v>779</v>
       </c>
-      <c r="B123" t="s">
-        <v>780</v>
-      </c>
       <c r="E123" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="F123" s="2" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="G123" s="2">
         <v>1972</v>
       </c>
       <c r="H123" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="I123" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="K123" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="L123" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="M123" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="N123" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="O123" t="s">
         <v>340</v>
       </c>
       <c r="S123" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="T123" t="s">
         <v>342</v>
       </c>
       <c r="U123" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="V123" t="s">
+        <v>740</v>
+      </c>
+      <c r="W123" t="s">
         <v>741</v>
       </c>
-      <c r="W123" t="s">
+      <c r="X123" t="s">
         <v>742</v>
-      </c>
-      <c r="X123" t="s">
-        <v>743</v>
       </c>
       <c r="AD123">
         <v>125</v>
@@ -16603,7 +16612,7 @@
         <v>340</v>
       </c>
       <c r="F124" s="2" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="G124" s="2">
         <v>1972</v>
@@ -16615,37 +16624,37 @@
         <v>344</v>
       </c>
       <c r="K124" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="L124" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="M124" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="N124" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="O124" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="S124" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="T124" t="s">
         <v>342</v>
       </c>
       <c r="U124" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="V124" t="s">
+        <v>740</v>
+      </c>
+      <c r="W124" t="s">
         <v>741</v>
       </c>
-      <c r="W124" t="s">
+      <c r="X124" t="s">
         <v>742</v>
-      </c>
-      <c r="X124" t="s">
-        <v>743</v>
       </c>
       <c r="AD124">
         <v>128</v>
@@ -16674,7 +16683,7 @@
         <v>257</v>
       </c>
       <c r="F125" s="2" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="G125" s="2">
         <v>1975</v>
@@ -16683,7 +16692,7 @@
         <v>77</v>
       </c>
       <c r="I125" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="J125" t="s">
         <v>36</v>
@@ -16879,7 +16888,7 @@
         <v>392</v>
       </c>
       <c r="F127" s="2" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="G127" s="2">
         <v>1978</v>
@@ -16992,7 +17001,7 @@
         <v>364</v>
       </c>
       <c r="F128" s="2" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="G128" s="2">
         <v>2000</v>
@@ -17105,7 +17114,7 @@
         <v>366</v>
       </c>
       <c r="F129" s="2" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="G129" s="2">
         <v>2002</v>
@@ -17197,55 +17206,55 @@
     </row>
     <row r="130" spans="1:37">
       <c r="A130" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="B130" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="C130" t="s">
         <v>89</v>
       </c>
       <c r="E130" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="F130" s="2" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="G130" s="2">
         <v>2006</v>
       </c>
       <c r="H130" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="I130" t="s">
         <v>340</v>
       </c>
       <c r="K130" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="P130" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="Q130" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="S130" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="T130" t="s">
         <v>342</v>
       </c>
       <c r="U130" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="V130" t="s">
+        <v>740</v>
+      </c>
+      <c r="W130" t="s">
         <v>741</v>
       </c>
-      <c r="W130" t="s">
+      <c r="X130" t="s">
         <v>742</v>
-      </c>
-      <c r="X130" t="s">
-        <v>743</v>
       </c>
       <c r="AD130">
         <v>127</v>
@@ -17259,55 +17268,55 @@
     </row>
     <row r="131" spans="1:37">
       <c r="A131" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="B131" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="C131" t="s">
         <v>124</v>
       </c>
       <c r="E131" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="F131" s="2" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G131" s="2">
         <v>2008</v>
       </c>
       <c r="H131" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="I131" t="s">
         <v>340</v>
       </c>
       <c r="K131" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="P131" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="Q131" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="S131" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="T131" t="s">
         <v>342</v>
       </c>
       <c r="U131" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="V131" t="s">
+        <v>740</v>
+      </c>
+      <c r="W131" t="s">
         <v>741</v>
       </c>
-      <c r="W131" t="s">
+      <c r="X131" t="s">
         <v>742</v>
-      </c>
-      <c r="X131" t="s">
-        <v>743</v>
       </c>
       <c r="AD131">
         <v>126</v>
@@ -17321,55 +17330,55 @@
     </row>
     <row r="132" spans="1:37">
       <c r="A132" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="B132" t="s">
+        <v>789</v>
+      </c>
+      <c r="C132" t="s">
+        <v>793</v>
+      </c>
+      <c r="E132" t="s">
         <v>790</v>
       </c>
-      <c r="C132" t="s">
-        <v>794</v>
-      </c>
-      <c r="E132" t="s">
-        <v>791</v>
-      </c>
       <c r="F132" s="2" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="G132" s="2">
         <v>2011</v>
       </c>
       <c r="H132" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="I132" t="s">
         <v>340</v>
       </c>
       <c r="K132" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="P132" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="Q132" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="S132" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="T132" t="s">
         <v>342</v>
       </c>
       <c r="U132" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="V132" t="s">
+        <v>740</v>
+      </c>
+      <c r="W132" t="s">
         <v>741</v>
       </c>
-      <c r="W132" t="s">
+      <c r="X132" t="s">
         <v>742</v>
-      </c>
-      <c r="X132" t="s">
-        <v>743</v>
       </c>
       <c r="AD132">
         <v>129</v>
@@ -17389,17 +17398,17 @@
         <v>478</v>
       </c>
       <c r="E133" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="F133"/>
       <c r="G133" s="2" t="s">
+        <v>843</v>
+      </c>
+      <c r="J133" t="s">
+        <v>841</v>
+      </c>
+      <c r="S133" t="s">
         <v>844</v>
-      </c>
-      <c r="J133" t="s">
-        <v>842</v>
-      </c>
-      <c r="S133" t="s">
-        <v>845</v>
       </c>
     </row>
     <row r="134" spans="1:37">

</xml_diff>